<commit_message>
added eidolon directory and index page links TODO: implement basic Eidolong game states
</commit_message>
<xml_diff>
--- a/public/images/dungeon/map/tileReference.xlsx
+++ b/public/images/dungeon/map/tileReference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="972" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -49,12 +50,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -513,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -667,7 +670,7 @@
         <v>44</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G5" s="18" t="n">
         <v>46</v>

</xml_diff>